<commit_message>
poprawienie formul w skrypcie
</commit_message>
<xml_diff>
--- a/lab3tt.xlsx
+++ b/lab3tt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\Digital_Technology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D93DD8-4DC2-4E36-87AB-4E35D3F83F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC9085D-9295-49C2-9463-5BA73F9F8213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AFE71B3F-7985-4110-92C2-D5CF060CC580}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFE71B3F-7985-4110-92C2-D5CF060CC580}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -189,20 +189,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -519,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8506AB-DE95-471D-BCB1-F29AD2A26170}">
   <dimension ref="B1:V45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,35 +539,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="O1" s="5" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5" t="s">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="5"/>
+      <c r="U1" s="4"/>
       <c r="V1" t="s">
         <v>18</v>
       </c>
@@ -1028,26 +1027,26 @@
       <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4" t="s">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4" t="s">
+      <c r="J22" s="5"/>
+      <c r="K22" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L22" s="4"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
@@ -1368,26 +1367,26 @@
       <c r="B36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
@@ -1436,12 +1435,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="G1:I1"/>
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="K36:L36"/>
@@ -1450,6 +1443,12 @@
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="K22:L22"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1460,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977A98DF-B4D9-425C-BA27-BC873EAD8974}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>